<commit_message>
Inserido mais arquivos *.html e *.pdf sobre python
</commit_message>
<xml_diff>
--- a/docs/python/html/Nº de páginas.xlsx
+++ b/docs/python/html/Nº de páginas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\html\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A305DEC4-136D-4C11-86D1-632B69A069A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51104B5C-82FF-446E-9832-5B11D1B307A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9705" yWindow="480" windowWidth="10605" windowHeight="8715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ambientes_virtuais_python</t>
   </si>
@@ -72,13 +72,31 @@
   </si>
   <si>
     <t>flask_extensions.html</t>
+  </si>
+  <si>
+    <t>Conceitos_de_Classes_em_Python</t>
+  </si>
+  <si>
+    <t>Extracao_de_Dados_com_Python</t>
+  </si>
+  <si>
+    <t>Extracao_de_Dados_em_Python</t>
+  </si>
+  <si>
+    <t>Lista_de_Dependencias_Python</t>
+  </si>
+  <si>
+    <t>Manipulacao_de_Planilhas_Excel_e_HTML_com_Python</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,8 +111,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -104,6 +128,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -120,12 +150,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -408,15 +447,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="58.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -521,6 +560,73 @@
         <v>179</v>
       </c>
     </row>
+    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="5">
+        <f>B13+B26</f>
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <f>SUM(B17:B25)</f>
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+ apostilas sobe python
</commit_message>
<xml_diff>
--- a/docs/python/html/Nº de páginas.xlsx
+++ b/docs/python/html/Nº de páginas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\html\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51104B5C-82FF-446E-9832-5B11D1B307A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F44FF25-A189-474A-8CB8-22C0DB574F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>ambientes_virtuais_python</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>python_project_structure_with_explanation</t>
   </si>
 </sst>
 </file>
@@ -450,7 +453,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,7 +569,7 @@
       </c>
       <c r="B15" s="5">
         <f>B13+B26</f>
-        <v>199</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -610,7 +613,12 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="1"/>
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
@@ -624,7 +632,7 @@
     <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <f>SUM(B17:B25)</f>
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ arquivos sobre python
</commit_message>
<xml_diff>
--- a/docs/python/html/Nº de páginas.xlsx
+++ b/docs/python/html/Nº de páginas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\html\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F44FF25-A189-474A-8CB8-22C0DB574F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81605AA6-FAB9-4103-BECB-4D931A0F67D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="135" yWindow="0" windowWidth="14295" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>ambientes_virtuais_python</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>python_project_structure_with_explanation</t>
+  </si>
+  <si>
+    <t>Exemplos_de_Caminho_de_Arquivos_em_Python</t>
+  </si>
+  <si>
+    <t>downloadArquivosNet</t>
   </si>
 </sst>
 </file>
@@ -452,8 +458,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +575,7 @@
       </c>
       <c r="B15" s="5">
         <f>B13+B26</f>
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -621,10 +627,20 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="1"/>
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
@@ -632,7 +648,7 @@
     <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <f>SUM(B17:B25)</f>
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alterado o caminhos das apostilas python
</commit_message>
<xml_diff>
--- a/docs/python/html/Nº de páginas.xlsx
+++ b/docs/python/html/Nº de páginas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\html\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81605AA6-FAB9-4103-BECB-4D931A0F67D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E199E6-ABE5-414F-90E5-03916E6DE1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="0" windowWidth="14295" windowHeight="11070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>ambientes_virtuais_python</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Conceitos_de_Classes_em_Python</t>
   </si>
   <si>
-    <t>Extracao_de_Dados_com_Python</t>
-  </si>
-  <si>
     <t>Extracao_de_Dados_em_Python</t>
   </si>
   <si>
@@ -99,6 +96,27 @@
   </si>
   <si>
     <t>downloadArquivosNet</t>
+  </si>
+  <si>
+    <t>conceitosDetalhadoComIndece+Explicacao</t>
+  </si>
+  <si>
+    <t>guia_extracao_de_dados_python</t>
+  </si>
+  <si>
+    <t>macetes_em_python</t>
+  </si>
+  <si>
+    <t>provedoresPython</t>
+  </si>
+  <si>
+    <t>requirementsxrailway.json</t>
+  </si>
+  <si>
+    <t>Conceitos_Avançados_em_Python</t>
+  </si>
+  <si>
+    <t>recursosAprenderPraticarPython</t>
   </si>
 </sst>
 </file>
@@ -122,12 +140,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFCE9178"/>
+      <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,6 +164,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -159,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -167,14 +191,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -456,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +493,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1">
@@ -476,7 +501,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
@@ -484,7 +509,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
@@ -492,7 +517,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1">
@@ -500,7 +525,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1">
@@ -508,7 +533,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1">
@@ -516,7 +541,7 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1">
@@ -524,7 +549,7 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1">
@@ -532,7 +557,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1">
@@ -540,7 +565,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1">
@@ -548,7 +573,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1">
@@ -556,99 +581,168 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
-        <f>SUM(B1:B12)</f>
-        <v>179</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <f>SUM(B1:B13)</f>
+        <v>195</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="4">
+        <f>B18+B39</f>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="5">
-        <f>B13+B26</f>
-        <v>208</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" s="1">
+      <c r="B27" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>20</v>
-      </c>
-      <c r="B23" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="1">
+      <c r="B29" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-    </row>
-    <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="2">
-        <f>SUM(B17:B25)</f>
-        <v>29</v>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="2">
+        <f>SUM(B22:B38)</f>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualizado apostilas sobre python
</commit_message>
<xml_diff>
--- a/docs/python/html/Nº de páginas.xlsx
+++ b/docs/python/html/Nº de páginas.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\html\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF807920-9369-4153-A5A8-E7A27A308687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90483DBE-E034-4642-9C1C-951D402A92CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21960" yWindow="585" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
     <sheet name="Planilha2" sheetId="3" r:id="rId3"/>
+    <sheet name="merged" sheetId="4" r:id="rId4"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="61">
   <si>
     <t>ambientes_virtuais_python</t>
   </si>
@@ -212,13 +216,114 @@
   </si>
   <si>
     <t>.pdf"</t>
+  </si>
+  <si>
+    <r>
+      <t>r</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD16969"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'D:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD16969"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>EUSSITESEPROJETOS\Sites</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD16969"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ortifolioDoMaia\docs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD16969"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ython</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD16969"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>df\separados</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFD7BA7D"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>\</t>
+    </r>
+  </si>
+  <si>
+    <t>Atribuicao_de_Multiplos_Valores</t>
+  </si>
+  <si>
+    <t>apostila_de_paythonI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +353,24 @@
     <font>
       <sz val="11"/>
       <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF569CD6"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD16969"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD7BA7D"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -296,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -321,6 +444,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -336,6 +463,278 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Plan1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Ambientes_Virtuais_no_Python</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>Aplicacao_de_Integracao_de_APIs_com_Flask</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>Apostila_do_Desenvolvedor_Python</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>conceiosDeMSQL</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>conceitoDeDicionarios</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>conceitosDeEntradaSaida</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>conceitosDeFuncoes</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>conceitosDeInsercaoDadosMSQL</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>conceitosDeListas</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>conceitosDeMatplotlib</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>conceitosDeModulos</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>conceitosDeSaida</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>conceitosDeSets</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>conceitosDeStrings</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>conceitosDeTuplas</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>conceitosDeVariaveis</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>conceitosGlossarios</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>Conceitos_Avancados_em_Python</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>Conceitos_Avançados_em_Python</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>Conceitos_Basicos_de_Python</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>Conceitos_de_Classes_em_Python</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>Conceitos_de_POO_em_Python</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>Cronograma_de_Estudo</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24" t="str">
+            <v>downloadArquivosNet</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25" t="str">
+            <v>Exemplos_de_Caminho_de_Arquivoscem_Python</v>
+          </cell>
+        </row>
+        <row r="26">
+          <cell r="A26" t="str">
+            <v>Exemplos_de_Caminho_de_Arquivos_em_Python</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="A27" t="str">
+            <v>Exemplo_de_requirements.txt_e_Explicacao_sobre_railway.json</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="A28" t="str">
+            <v>Extensoes_Populares_do_Flask</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="A29" t="str">
+            <v>Extracao_de_Dados_com_Python</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30" t="str">
+            <v>Extracao_de_Dados_em_Python</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31" t="str">
+            <v>Funcoes_Especiais_em_Python</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32" t="str">
+            <v>guia_extracao_de_dados_python</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33" t="str">
+            <v>Lista_de_Dependencias_Python</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34" t="str">
+            <v>Macetes_em_Python</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35" t="str">
+            <v>Manipulacao_de_Planilhas_Excel_e_HTML_com_Python</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36" t="str">
+            <v>Mapa_do_Python</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37" t="str">
+            <v>menipulacaoDeArquivos</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38" t="str">
+            <v>Principais_Provedores_de_Hospedagem_para_Python</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39" t="str">
+            <v>Problemas_Resolvidos_em_Python</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40" t="str">
+            <v>provedoresPython</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41" t="str">
+            <v>Python_Project_Structure</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="A42" t="str">
+            <v>python_project_structure_with_explanation</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="A43" t="str">
+            <v>Recursos_para_Aprender_e _raticar_Python</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="A44" t="str">
+            <v>recusrosAprenderPraticarPython</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45" t="str">
+            <v>requirementsxrailway.json</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46" t="str">
+            <v>Resumo_de_Assuntos_Avancados_em_Desenvolvimento_Web_com_Python_Codigos</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47" t="str">
+            <v>Resumo_de_Assuntos_Avançados_em_Desenvolvimento_Webcom_Python_Explicacao</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48" t="str">
+            <v>Resumo_de_Assuntos_Avançados_em_Desenvolvimento_Web_com_Python</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49" t="str">
+            <v>Sites_para_Deployment</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50" t="str">
+            <v>termosFundamentais</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51" t="str">
+            <v>tutorial_manipulacao_python</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -601,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,8 +1138,8 @@
         <v>15</v>
       </c>
       <c r="B20" s="4">
-        <f>B18+B53</f>
-        <v>310</v>
+        <f>B18+B57</f>
+        <v>315</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -976,15 +1375,37 @@
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="1"/>
+      <c r="A51" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="1">
+        <v>2</v>
+      </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="1"/>
-    </row>
-    <row r="53" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B53" s="2">
-        <f>SUM(B22:B52)</f>
-        <v>115</v>
+      <c r="A52" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B57" s="2">
+        <f>SUM(B22:B56)</f>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -994,10 +1415,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73051E8E-B662-4F87-87B0-53E0075DF285}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2159,6 +2580,422 @@
         <v>48</v>
       </c>
     </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -2168,8 +3005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E716244-892B-44E9-8A6A-67CC860B2FA3}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD17"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2764,4 +3601,796 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953DA6B0-9276-42EC-92CB-AF2879D03A8B}">
+  <dimension ref="A1:D51"/>
+  <sheetViews>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="str">
+        <f>Planilha1!B1</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B1" t="str">
+        <f>[1]Plan1!$A1</f>
+        <v>Ambientes_Virtuais_no_Python</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="str">
+        <f>Planilha1!B2</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B2" t="str">
+        <f>[1]Plan1!$A2</f>
+        <v>Aplicacao_de_Integracao_de_APIs_com_Flask</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="str">
+        <f>Planilha1!B3</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B3" t="str">
+        <f>[1]Plan1!$A3</f>
+        <v>Apostila_do_Desenvolvedor_Python</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="str">
+        <f>Planilha1!B4</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B4" t="str">
+        <f>[1]Plan1!$A4</f>
+        <v>conceiosDeMSQL</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="str">
+        <f>Planilha1!B5</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B5" t="str">
+        <f>[1]Plan1!$A5</f>
+        <v>conceitoDeDicionarios</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="str">
+        <f>Planilha1!B6</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B6" t="str">
+        <f>[1]Plan1!$A6</f>
+        <v>conceitosDeEntradaSaida</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="str">
+        <f>Planilha1!B7</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B7" t="str">
+        <f>[1]Plan1!$A7</f>
+        <v>conceitosDeFuncoes</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="str">
+        <f>[1]Plan1!$A8</f>
+        <v>conceitosDeInsercaoDadosMSQL</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="str">
+        <f>Planilha1!B9</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B9" t="str">
+        <f>[1]Plan1!$A9</f>
+        <v>conceitosDeListas</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="str">
+        <f>Planilha1!B10</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B10" t="str">
+        <f>[1]Plan1!$A10</f>
+        <v>conceitosDeMatplotlib</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="str">
+        <f>Planilha1!B11</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B11" t="str">
+        <f>[1]Plan1!$A11</f>
+        <v>conceitosDeModulos</v>
+      </c>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="str">
+        <f>Planilha1!B12</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B12" t="str">
+        <f>[1]Plan1!$A12</f>
+        <v>conceitosDeSaida</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="str">
+        <f>Planilha1!B13</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B13" t="str">
+        <f>[1]Plan1!$A13</f>
+        <v>conceitosDeSets</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="str">
+        <f>Planilha1!B14</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B14" t="str">
+        <f>[1]Plan1!$A14</f>
+        <v>conceitosDeStrings</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="str">
+        <f>Planilha1!B15</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B15" t="str">
+        <f>[1]Plan1!$A15</f>
+        <v>conceitosDeTuplas</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="str">
+        <f>Planilha1!B16</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B16" t="str">
+        <f>[1]Plan1!$A16</f>
+        <v>conceitosDeVariaveis</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="str">
+        <f>Planilha1!B17</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B17" t="str">
+        <f>[1]Plan1!$A17</f>
+        <v>conceitosGlossarios</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="str">
+        <f>Planilha1!B18</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B18" t="str">
+        <f>[1]Plan1!$A18</f>
+        <v>Conceitos_Avancados_em_Python</v>
+      </c>
+      <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="str">
+        <f>Planilha1!B19</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B19" t="str">
+        <f>[1]Plan1!$A19</f>
+        <v>Conceitos_Avançados_em_Python</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="str">
+        <f>Planilha1!B20</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B20" t="str">
+        <f>[1]Plan1!$A20</f>
+        <v>Conceitos_Basicos_de_Python</v>
+      </c>
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="str">
+        <f>Planilha1!B21</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B21" t="str">
+        <f>[1]Plan1!$A21</f>
+        <v>Conceitos_de_Classes_em_Python</v>
+      </c>
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="str">
+        <f>Planilha1!B22</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B22" t="str">
+        <f>[1]Plan1!$A22</f>
+        <v>Conceitos_de_POO_em_Python</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="str">
+        <f>Planilha1!B23</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B23" t="str">
+        <f>[1]Plan1!$A23</f>
+        <v>Cronograma_de_Estudo</v>
+      </c>
+      <c r="C23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="str">
+        <f>Planilha1!B24</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B24" t="str">
+        <f>[1]Plan1!$A24</f>
+        <v>downloadArquivosNet</v>
+      </c>
+      <c r="C24" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="str">
+        <f>Planilha1!B25</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B25" t="str">
+        <f>[1]Plan1!$A25</f>
+        <v>Exemplos_de_Caminho_de_Arquivoscem_Python</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="str">
+        <f>Planilha1!B26</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B26" t="str">
+        <f>[1]Plan1!$A26</f>
+        <v>Exemplos_de_Caminho_de_Arquivos_em_Python</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="str">
+        <f>Planilha1!B27</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B27" t="str">
+        <f>[1]Plan1!$A27</f>
+        <v>Exemplo_de_requirements.txt_e_Explicacao_sobre_railway.json</v>
+      </c>
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="str">
+        <f>Planilha1!B28</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B28" t="str">
+        <f>[1]Plan1!$A28</f>
+        <v>Extensoes_Populares_do_Flask</v>
+      </c>
+      <c r="C28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="str">
+        <f>Planilha1!B29</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B29" t="str">
+        <f>[1]Plan1!$A29</f>
+        <v>Extracao_de_Dados_com_Python</v>
+      </c>
+      <c r="C29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="str">
+        <f>Planilha1!B30</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B30" t="str">
+        <f>[1]Plan1!$A30</f>
+        <v>Extracao_de_Dados_em_Python</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="str">
+        <f>Planilha1!B31</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B31" t="str">
+        <f>[1]Plan1!$A31</f>
+        <v>Funcoes_Especiais_em_Python</v>
+      </c>
+      <c r="C31" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="str">
+        <f>Planilha1!B32</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B32" t="str">
+        <f>[1]Plan1!$A32</f>
+        <v>guia_extracao_de_dados_python</v>
+      </c>
+      <c r="C32" t="s">
+        <v>43</v>
+      </c>
+      <c r="D32" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="str">
+        <f>Planilha1!B33</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B33" t="str">
+        <f>[1]Plan1!$A33</f>
+        <v>Lista_de_Dependencias_Python</v>
+      </c>
+      <c r="C33" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="str">
+        <f>Planilha1!B34</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B34" t="str">
+        <f>[1]Plan1!$A34</f>
+        <v>Macetes_em_Python</v>
+      </c>
+      <c r="C34" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="str">
+        <f>Planilha1!B35</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B35" t="str">
+        <f>[1]Plan1!$A35</f>
+        <v>Manipulacao_de_Planilhas_Excel_e_HTML_com_Python</v>
+      </c>
+      <c r="C35" t="s">
+        <v>43</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f>Planilha1!B36</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B36" t="str">
+        <f>[1]Plan1!$A36</f>
+        <v>Mapa_do_Python</v>
+      </c>
+      <c r="C36" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="str">
+        <f>Planilha1!B37</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B37" t="str">
+        <f>[1]Plan1!$A37</f>
+        <v>menipulacaoDeArquivos</v>
+      </c>
+      <c r="C37" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="str">
+        <f>Planilha1!B38</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B38" t="str">
+        <f>[1]Plan1!$A38</f>
+        <v>Principais_Provedores_de_Hospedagem_para_Python</v>
+      </c>
+      <c r="C38" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f>Planilha1!B39</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B39" t="str">
+        <f>[1]Plan1!$A39</f>
+        <v>Problemas_Resolvidos_em_Python</v>
+      </c>
+      <c r="C39" t="s">
+        <v>43</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="str">
+        <f>Planilha1!B40</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B40" t="str">
+        <f>[1]Plan1!$A40</f>
+        <v>provedoresPython</v>
+      </c>
+      <c r="C40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="str">
+        <f>Planilha1!B41</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B41" t="str">
+        <f>[1]Plan1!$A41</f>
+        <v>Python_Project_Structure</v>
+      </c>
+      <c r="C41" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="str">
+        <f>Planilha1!B42</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B42" t="str">
+        <f>[1]Plan1!$A42</f>
+        <v>python_project_structure_with_explanation</v>
+      </c>
+      <c r="C42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="str">
+        <f>Planilha1!B43</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B43" t="str">
+        <f>[1]Plan1!$A43</f>
+        <v>Recursos_para_Aprender_e _raticar_Python</v>
+      </c>
+      <c r="C43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="str">
+        <f>Planilha1!B44</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B44" t="str">
+        <f>[1]Plan1!$A44</f>
+        <v>recusrosAprenderPraticarPython</v>
+      </c>
+      <c r="C44" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="str">
+        <f>Planilha1!B45</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B45" t="str">
+        <f>[1]Plan1!$A45</f>
+        <v>requirementsxrailway.json</v>
+      </c>
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="str">
+        <f>Planilha1!B46</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B46" t="str">
+        <f>[1]Plan1!$A46</f>
+        <v>Resumo_de_Assuntos_Avancados_em_Desenvolvimento_Web_com_Python_Codigos</v>
+      </c>
+      <c r="C46" t="s">
+        <v>43</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="str">
+        <f>Planilha1!B47</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B47" t="str">
+        <f>[1]Plan1!$A47</f>
+        <v>Resumo_de_Assuntos_Avançados_em_Desenvolvimento_Webcom_Python_Explicacao</v>
+      </c>
+      <c r="C47" t="s">
+        <v>43</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="str">
+        <f>Planilha1!B48</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B48" t="str">
+        <f>[1]Plan1!$A48</f>
+        <v>Resumo_de_Assuntos_Avançados_em_Desenvolvimento_Web_com_Python</v>
+      </c>
+      <c r="C48" t="s">
+        <v>43</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="str">
+        <f>Planilha1!B49</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B49" t="str">
+        <f>[1]Plan1!$A49</f>
+        <v>Sites_para_Deployment</v>
+      </c>
+      <c r="C49" t="s">
+        <v>43</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="str">
+        <f>Planilha1!B50</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B50" t="str">
+        <f>[1]Plan1!$A50</f>
+        <v>termosFundamentais</v>
+      </c>
+      <c r="C50" t="s">
+        <v>43</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="str">
+        <f>Planilha1!B51</f>
+        <v>D:\MEUSSITESEPROJETOS\Sites\portifolioDoMaia\docs\python\htmll\PrintYet\</v>
+      </c>
+      <c r="B51" t="str">
+        <f>[1]Plan1!$A51</f>
+        <v>tutorial_manipulacao_python</v>
+      </c>
+      <c r="C51" t="s">
+        <v>43</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>